<commit_message>
Updtae spreadsheet with if-then-else example.
</commit_message>
<xml_diff>
--- a/abs_int.xlsx
+++ b/abs_int.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorj/abs_int/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326C1FDE-0527-EE4E-8321-70C1C39D4F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1342B2B7-03CF-FA4D-B588-76C99C33442F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8340" yWindow="1920" windowWidth="31560" windowHeight="25120" activeTab="4" xr2:uid="{539FF1CB-7311-1346-AD43-E4613586CF79}"/>
+    <workbookView xWindow="8320" yWindow="1980" windowWidth="31560" windowHeight="25120" activeTab="5" xr2:uid="{539FF1CB-7311-1346-AD43-E4613586CF79}"/>
   </bookViews>
   <sheets>
     <sheet name="swap-ok" sheetId="6" r:id="rId1"/>
     <sheet name="swap-bad-2" sheetId="4" r:id="rId2"/>
     <sheet name="swap-bad" sheetId="2" r:id="rId3"/>
     <sheet name="ite-swap-ok" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
-    <sheet name="ite-swap-bad-1" sheetId="7" r:id="rId6"/>
+    <sheet name="max-1" sheetId="8" r:id="rId5"/>
+    <sheet name="ifeif-max" sheetId="9" r:id="rId6"/>
+    <sheet name="ite-swap-bad-1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="258">
   <si>
     <t>procedure Swap  (X : in out Integer; Y : in out Integer) is</t>
   </si>
@@ -551,13 +552,277 @@
   </si>
   <si>
     <t xml:space="preserve">   end Max_X;</t>
+  </si>
+  <si>
+    <t>1, 3</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Undefined, (1, 3), Undefined, (1, 3)))</t>
+  </si>
+  <si>
+    <t>Formal out parameter, Same, is Undefined</t>
+  </si>
+  <si>
+    <t>Io_Param  (X, (1, 1))</t>
+  </si>
+  <si>
+    <t>Ou_Param (Same, (1, 3))</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Undefined, (2, 1), Undefined, (2, 1)))</t>
+  </si>
+  <si>
+    <t>4, 1</t>
+  </si>
+  <si>
+    <t>Read (Y, 4, 2))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (1, 1)), (Read, (4, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2)), Read, (4, 2)))</t>
+  </si>
+  <si>
+    <t>Assign (Same, (5, 1))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (5, 1), Defined, (5, 1)))</t>
+  </si>
+  <si>
+    <t>Mark and keep because of conditional code</t>
+  </si>
+  <si>
+    <t>4 &amp; 2</t>
+  </si>
+  <si>
+    <t>6, 1</t>
+  </si>
+  <si>
+    <t>Declare (Temp,(2, 1))</t>
+  </si>
+  <si>
+    <t>Read (Y, (6, 2))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (1, 1)), (Read, (6, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2)), Read, (6, 2)))</t>
+  </si>
+  <si>
+    <t>Immediately predeing statement is 4</t>
+  </si>
+  <si>
+    <t>7, 1</t>
+  </si>
+  <si>
+    <t>6, 2</t>
+  </si>
+  <si>
+    <t>7, 2</t>
+  </si>
+  <si>
+    <t>Read (X, (7, 1))</t>
+  </si>
+  <si>
+    <t>Assign (Temp, (7, 2))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (1, 1)), (Read, (7, 1)))</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Defined, (7, 2), Defined, (7, 2)))</t>
+  </si>
+  <si>
+    <t>8, 2</t>
+  </si>
+  <si>
+    <t>Assign (X, (8, 2))</t>
+  </si>
+  <si>
+    <t>Read (Y, (8, 1))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2)), Read, (8, 2)))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (8, 2)), (Defined, (8, 2)))</t>
+  </si>
+  <si>
+    <t>7 &amp; 8</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Defined, (7, 2), Read, (9, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (9, 2)), Defined, (9, 2)))</t>
+  </si>
+  <si>
+    <t>Assign (Same, (10, 1))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (10, 1), Defined, (10, 1)))</t>
+  </si>
+  <si>
+    <t>12, 1</t>
+  </si>
+  <si>
+    <t>Assign (Same, (12, 1))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (12, 1), Defined, (12, 1)))</t>
+  </si>
+  <si>
+    <t>6 &amp; 12</t>
+  </si>
+  <si>
+    <t>Immediately preceding statement is 6</t>
+  </si>
+  <si>
+    <t>Statement 4 abstracion no longer needed</t>
+  </si>
+  <si>
+    <t>Statement 6 abstracion no longer needed</t>
+  </si>
+  <si>
+    <t>13, 1</t>
+  </si>
+  <si>
+    <t>End_If</t>
+  </si>
+  <si>
+    <t>Merge different branches of if statement</t>
+  </si>
+  <si>
+    <t>5  &amp; 10 &amp; 12</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (9, 2)), Read, (6, 2)))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (8, 2)), (Read, (6, 1)))</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Undefined, (2, 1), Read, (9, 1)))</t>
+  </si>
+  <si>
+    <t>14, 1</t>
+  </si>
+  <si>
+    <t>14, 2</t>
+  </si>
+  <si>
+    <t>14, 3</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (8, 2)), (Read, (14, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (9, 2)), Read, (14, 2)))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (12, 1), Read, (14, 3)))</t>
+  </si>
+  <si>
+    <t>13 &amp; 14</t>
+  </si>
+  <si>
+    <t>In out fomal X both read and assigned</t>
+  </si>
+  <si>
+    <t>In out fomal, Y, both read and assigned</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (8, 2)), Read, (14, 1)))</t>
+  </si>
+  <si>
+    <t>Out formal, Same, assigned and read</t>
+  </si>
+  <si>
+    <t>Temp only defined and read on some paths</t>
+  </si>
+  <si>
+    <t>No Issues</t>
+  </si>
+  <si>
+    <t>Io_Param (X, (14, 1))</t>
+  </si>
+  <si>
+    <t>Io_Param (Y, (14, 2))</t>
+  </si>
+  <si>
+    <t>Ou_Param (Same, (14, 3))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      elsif X = Y then</t>
+  </si>
+  <si>
+    <t>11, 1</t>
+  </si>
+  <si>
+    <t>Read (X, (11, 1))</t>
+  </si>
+  <si>
+    <t>Read (Y, (11, 2))</t>
+  </si>
+  <si>
+    <t>6 &amp; 11</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (1, 1)), (Read, (11, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2)), Read, (11, 2)))</t>
+  </si>
+  <si>
+    <t>11 &amp; 12</t>
+  </si>
+  <si>
+    <t>Null_Else</t>
+  </si>
+  <si>
+    <t>11 &amp; 13</t>
+  </si>
+  <si>
+    <t>5  &amp; 10 &amp; 13</t>
+  </si>
+  <si>
+    <t>13, 2</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (8, 2)), (Read, (11, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (9, 2)), Read, (11, 2)))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Undefined, (1, 3), Defined, (10, 1)))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Undefined, (1, 3), Read, (14, 3)))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* The out parameter,  Same , may not be assigned a value </t>
+  </si>
+  <si>
+    <t>Simple model of definedness cann ot determine the null else branch is non-executable.</t>
+  </si>
+  <si>
+    <t>* Out formal, Same, may not have a valid value.  It may have not been assigned.</t>
+  </si>
+  <si>
+    <t>Immediately predeing statement is 6</t>
+  </si>
+  <si>
+    <t>Saved states from 5, 10, 13 no longer required</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -604,6 +869,26 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -625,7 +910,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -633,6 +918,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1932,10 +2220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD2435B-A905-DA40-ADC9-DCD4C89B1191}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C2" sqref="C2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2319,13 +2607,6 @@
     <row r="55" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F55" s="6"/>
     </row>
-    <row r="65" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2333,86 +2614,664 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF102DA-B60A-D24C-B90A-54700D02483D}">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="22.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C14" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F18" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C34" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F36" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F37" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F38" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>8</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F44" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F45" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F46" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>9</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F50" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F51" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>10</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F54" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F55" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F56" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>11</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>12</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C60" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F61" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E62" s="9"/>
+      <c r="F62" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F63" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F64" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>13</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C66" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F67" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F68" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F69" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F70" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>14</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>169</v>
       </c>
+      <c r="C72" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F73" s="9"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C74" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F75" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F76" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F77" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F78" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H79" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F82" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2420,8 +3279,760 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BA9936-B466-0545-AB32-7663543D1B16}">
+  <dimension ref="A1:H94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="22.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F18" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F22" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F23" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F24" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>6</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>7</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F36" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F37" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F38" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>8</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C42" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F43" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F44" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F45" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F46" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>9</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C49" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F50" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F51" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>10</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F54" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F55" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F56" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="2">
+        <v>11</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D59" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F60" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F61" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F62" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F63" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>12</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F67" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E68" s="9"/>
+      <c r="F68" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F69" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F70" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="2">
+        <v>13</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F73" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F74" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F75" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F76" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C78" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F79" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F80" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F81" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F82" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="2">
+        <v>14</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C85" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F85" s="9"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C86" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F87" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F88" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F89" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F90" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H92" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F94" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48821AE3-9308-7740-A704-CD4166125DE4}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView zoomScale="124" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
@@ -2834,19 +4445,9 @@
     <row r="62" spans="1:8" ht="14" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:8" ht="14" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:8" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="65" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="66" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="67" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="68" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="69" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="70" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="71" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="72" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="73" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="74" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="75" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="76" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
-    <row r="77" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="14" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="14" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add case statement analysis.
</commit_message>
<xml_diff>
--- a/abs_int.xlsx
+++ b/abs_int.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trevorj/abs_int/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1342B2B7-03CF-FA4D-B588-76C99C33442F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7853B30-B7D3-494E-9C8D-DB71204B08E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8320" yWindow="1980" windowWidth="31560" windowHeight="25120" activeTab="5" xr2:uid="{539FF1CB-7311-1346-AD43-E4613586CF79}"/>
+    <workbookView xWindow="8320" yWindow="1980" windowWidth="31560" windowHeight="25120" activeTab="4" xr2:uid="{539FF1CB-7311-1346-AD43-E4613586CF79}"/>
   </bookViews>
   <sheets>
     <sheet name="swap-ok" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="336">
   <si>
     <t>procedure Swap  (X : in out Integer; Y : in out Integer) is</t>
   </si>
@@ -542,9 +542,6 @@
     <t xml:space="preserve">         Y := Temp;</t>
   </si>
   <si>
-    <t xml:space="preserve">      else</t>
-  </si>
-  <si>
     <t xml:space="preserve">         Same := True;</t>
   </si>
   <si>
@@ -674,9 +671,6 @@
     <t>(Same, Pou, (Defined, (12, 1), Defined, (12, 1)))</t>
   </si>
   <si>
-    <t>6 &amp; 12</t>
-  </si>
-  <si>
     <t>Immediately preceding statement is 6</t>
   </si>
   <si>
@@ -695,15 +689,6 @@
     <t>Merge different branches of if statement</t>
   </si>
   <si>
-    <t>5  &amp; 10 &amp; 12</t>
-  </si>
-  <si>
-    <t>(Y, Pio, (Defined, (9, 2)), Read, (6, 2)))</t>
-  </si>
-  <si>
-    <t>(X, Pio, (Defined, (8, 2)), (Read, (6, 1)))</t>
-  </si>
-  <si>
     <t>(Temp, Lrw, (Undefined, (2, 1), Read, (9, 1)))</t>
   </si>
   <si>
@@ -816,6 +801,255 @@
   </si>
   <si>
     <t>Saved states from 5, 10, 13 no longer required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Sign : Integer;</t>
+  </si>
+  <si>
+    <t>Declare (Sign, (3, 1))</t>
+  </si>
+  <si>
+    <t>(Sign, Lrw, (Undefined, (3, 1), Undefined, (3, 1)))</t>
+  </si>
+  <si>
+    <t>2 &amp; 3</t>
+  </si>
+  <si>
+    <t>Read (X, (5, 1))</t>
+  </si>
+  <si>
+    <t>Read (Y, 5, 2))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2)), Read, (5, 2)))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (1, 1)), (Read, 5, 1)))</t>
+  </si>
+  <si>
+    <t>5 &amp; 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sign := 1;</t>
+  </si>
+  <si>
+    <t>Assign (Sign, (6, 1))</t>
+  </si>
+  <si>
+    <t>(Sign, Lrw, (Defined, (6, 1), Defined, (6, 1)))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2)), Read, (7, 2)))</t>
+  </si>
+  <si>
+    <t>5 &amp; 7</t>
+  </si>
+  <si>
+    <t>Immediately predeing statement is 5</t>
+  </si>
+  <si>
+    <t>Statement 5 abstracion no longer needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Sign := -1;</t>
+  </si>
+  <si>
+    <t>Assign (Sign, (8, 1))</t>
+  </si>
+  <si>
+    <t>(Sign, Lrw, (Defined, (8, 1), Defined (8, 1)))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else</t>
+  </si>
+  <si>
+    <t>Assign (Sign, (10, 1))</t>
+  </si>
+  <si>
+    <t>(Sign, Lrw, (Defined, (10, 1), Defined (10, 1)))</t>
+  </si>
+  <si>
+    <t>Immediately predeing statement is 7</t>
+  </si>
+  <si>
+    <t>Statement 7 abstracion no longer needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   end if;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Sign := 0;</t>
+  </si>
+  <si>
+    <t>7 &amp; 9</t>
+  </si>
+  <si>
+    <t>6 &amp; 8 &amp; 10</t>
+  </si>
+  <si>
+    <t>Merge 3 branches of if statement</t>
+  </si>
+  <si>
+    <t>Merge Conditions of if statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  case Sign is</t>
+  </si>
+  <si>
+    <t>Statement abstractions 6, 8, 10 no longer required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  when 1 =&gt;</t>
+  </si>
+  <si>
+    <t>Choices can only be static expressions</t>
+  </si>
+  <si>
+    <t>No changes to abstract state of definednes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Same := False;</t>
+  </si>
+  <si>
+    <t>Assign (Same, (14, 1))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (14, 1), Defined, (14, 1)))</t>
+  </si>
+  <si>
+    <t>(Sign, Lrw, (Read, (Defined, (10, 1), Read (12, 1)))</t>
+  </si>
+  <si>
+    <t>12 &amp; 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  when -1 =&gt;</t>
+  </si>
+  <si>
+    <t>16, 1</t>
+  </si>
+  <si>
+    <t>Read (X, (16, 1))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (1, 1)), (Read, (16, 1)))</t>
+  </si>
+  <si>
+    <t>16, 2</t>
+  </si>
+  <si>
+    <t>Assign (Temp, (12, 2))</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Defined, (16, 2), Defined, (16, 2)))</t>
+  </si>
+  <si>
+    <t>17, 1</t>
+  </si>
+  <si>
+    <t>Read (Y, (17, 1))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (1, 2), Read (17, 1)))</t>
+  </si>
+  <si>
+    <t>17, 2</t>
+  </si>
+  <si>
+    <t>(Assign, (X, (17, 2))</t>
+  </si>
+  <si>
+    <t>(X, Pio, (Defined, (17, 2), Defined (17, 2)))</t>
+  </si>
+  <si>
+    <t>16 &amp; 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Y := Temp;</t>
+  </si>
+  <si>
+    <t>18, 1</t>
+  </si>
+  <si>
+    <t>Read (Tenp, (18, 1))</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Defined, (16, 2), Read, (18, 1)))</t>
+  </si>
+  <si>
+    <t>18, 2</t>
+  </si>
+  <si>
+    <t>Assign (Y, (18, 2))</t>
+  </si>
+  <si>
+    <t>(Y, Pio, (Defined, (18, 2), Defined, (18, 2)))</t>
+  </si>
+  <si>
+    <t>17 &amp; 18</t>
+  </si>
+  <si>
+    <t>19, 1</t>
+  </si>
+  <si>
+    <t>Assign (Same, (19, 1))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (19, 1), Defined, (19, 1)))</t>
+  </si>
+  <si>
+    <t>when others =&gt;</t>
+  </si>
+  <si>
+    <t>18 &amp; 19</t>
+  </si>
+  <si>
+    <t>Immediately preceding statement 12</t>
+  </si>
+  <si>
+    <t>12 &amp; 16</t>
+  </si>
+  <si>
+    <t>12 &amp; 19</t>
+  </si>
+  <si>
+    <t>end case;</t>
+  </si>
+  <si>
+    <t>End_Case</t>
+  </si>
+  <si>
+    <t>21, 1</t>
+  </si>
+  <si>
+    <t>Assign (Same, (21, 1))</t>
+  </si>
+  <si>
+    <t>(Same, Pou, (Defined, (21, 1), Defined, (21, 1)))</t>
+  </si>
+  <si>
+    <t>22, 1</t>
+  </si>
+  <si>
+    <t>14 &amp; 19 &amp; 21</t>
+  </si>
+  <si>
+    <t>Merge different branches of case statement</t>
+  </si>
+  <si>
+    <t>(Temp, Lrw, (Undefined, (2, 1), Read, (18, 1)))</t>
+  </si>
+  <si>
+    <t>Stament abstractions 14, 19, 21 no longer needed</t>
+  </si>
+  <si>
+    <t>Read (Sign, (12, 1))</t>
+  </si>
+  <si>
+    <t>(Sign, Lrw, (Defined, (10, 1), Read (12, 1)))</t>
+  </si>
+  <si>
+    <t>end Max_X;</t>
   </si>
 </sst>
 </file>
@@ -2614,10 +2848,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDF102DA-B60A-D24C-B90A-54700D02483D}">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:H147"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2666,7 +2900,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>65</v>
@@ -2691,16 +2925,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2714,10 +2948,10 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2735,12 +2969,12 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F9" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F10" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2748,530 +2982,938 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>159</v>
+        <v>253</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <v>4</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>178</v>
+      <c r="F14" s="9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D15" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>179</v>
+      <c r="F15" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F16" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F17" s="2" t="s">
-        <v>179</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F18" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F19" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>182</v>
+      <c r="A18" s="2">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>5</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>181</v>
+        <v>258</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F22" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>48</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F24" s="9" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F25" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F26" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>6</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>262</v>
+      </c>
       <c r="C28" s="2" t="s">
-        <v>191</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>188</v>
+        <v>263</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F29" s="2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>189</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F30" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F31" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F32" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F33" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>7</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="C35" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F36" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C36" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F37" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F38" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F39" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+        <v>194</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F38" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F39" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F40" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F41" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>8</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B43" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F44" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F43" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F44" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F45" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F46" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F45" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F46" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F47" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F48" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
         <v>9</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C49" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F50" s="9" t="s">
-        <v>171</v>
+      <c r="B50" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F51" s="2" t="s">
-        <v>203</v>
+        <v>194</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F52" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>10</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>153</v>
+      <c r="F53" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F54" s="2" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F55" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F56" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>182</v>
+      <c r="F55" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="2">
+        <v>10</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
-        <v>11</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>166</v>
+      <c r="F58" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F59" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
-        <v>12</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>209</v>
+      <c r="F60" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F61" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>211</v>
+        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E62" s="9"/>
       <c r="F62" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F63" s="9" t="s">
-        <v>209</v>
+        <v>274</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F64" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>182</v>
+      <c r="A64" s="2">
+        <v>11</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F65" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="2">
-        <v>13</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>215</v>
+      <c r="F66" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F67" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>216</v>
+      <c r="F67" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F68" s="2" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F69" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F70" s="2" t="s">
-        <v>220</v>
+      <c r="F69" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>12</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="2">
-        <v>14</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>224</v>
+      <c r="F72" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C73" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F73" s="9"/>
+      <c r="F73" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C74" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>226</v>
+      <c r="F74" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F75" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>228</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F76" s="2" t="s">
-        <v>225</v>
+        <v>334</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F77" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>231</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F78" s="2" t="s">
-        <v>220</v>
+      <c r="A78" s="2">
+        <v>13</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>285</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H79" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F82" s="9"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="2">
+        <v>14</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F82" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F83" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F84" s="9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F85" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F86" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>15</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="E88" s="9"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H89" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>16</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C91" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F92" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F93" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F94" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F95" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F96" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>17</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C99" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F100" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F101" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F102" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F103" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F104" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>18</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C107" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F108" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F109" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F110" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F111" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F112" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>19</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F115" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F116" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F117" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F118" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F119" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>20</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>21</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E123" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F124" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F125" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F126" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F127" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F128" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="H128" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="2">
+        <v>22</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F131" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H131" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F132" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F133" s="9" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F134" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F135" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="2">
+        <v>23</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C137" s="2">
+        <v>23</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C138" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="F138" s="9"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G139" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F140" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F141" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F142" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F143" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H143" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F144" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="147" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F147" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3282,7 +3924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BA9936-B466-0545-AB32-7663543D1B16}">
   <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -3332,7 +3974,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>65</v>
@@ -3357,16 +3999,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -3380,10 +4022,10 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -3401,12 +4043,12 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F9" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F10" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -3425,47 +4067,47 @@
         <v>160</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D15" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F16" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F17" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F18" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F19" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -3479,15 +4121,15 @@
         <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>180</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F22" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>48</v>
@@ -3495,20 +4137,20 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F24" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F25" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -3519,56 +4161,56 @@
         <v>162</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>107</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F29" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>139</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F30" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F31" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F32" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -3579,29 +4221,29 @@
         <v>163</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F36" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>50</v>
@@ -3609,17 +4251,17 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F37" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F38" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F39" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3633,44 +4275,44 @@
         <v>31</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F43" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F44" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F45" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F46" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -3687,10 +4329,10 @@
         <v>140</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>132</v>
@@ -3704,20 +4346,20 @@
         <v>141</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F50" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F51" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -3731,13 +4373,13 @@
         <v>143</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E53" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>206</v>
-      </c>
       <c r="F53" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>153</v>
@@ -3745,20 +4387,20 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F54" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F55" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F56" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -3766,53 +4408,53 @@
         <v>11</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D59" s="2" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F60" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F61" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F62" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F63" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -3820,46 +4462,46 @@
         <v>12</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F67" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E68" s="9"/>
       <c r="F68" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F69" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F70" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -3867,76 +4509,76 @@
         <v>13</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F73" s="2" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F74" s="2" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F75" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F76" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F79" s="2" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F80" s="2" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F81" s="9" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F82" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -3944,82 +4586,82 @@
         <v>14</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F85" s="9"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F87" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H87" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F88" s="2" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F89" s="9" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F90" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H92" s="2" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>